<commit_message>
partial redrawing of sliders
</commit_message>
<xml_diff>
--- a/Algorithm to control changes in weight.xlsx
+++ b/Algorithm to control changes in weight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="15" r:id="rId1"/>
@@ -737,9 +737,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -749,12 +746,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -776,6 +767,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,7 +1271,7 @@
       <c r="E3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G3" t="s">
@@ -2647,7 +2647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -2709,7 +2709,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="40" t="s">
         <v>73</v>
       </c>
       <c r="C12" t="s">
@@ -2717,7 +2717,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="40" t="s">
         <v>72</v>
       </c>
       <c r="C13" t="s">
@@ -3356,33 +3356,33 @@
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="30"/>
+      <c r="W1" s="42"/>
     </row>
     <row r="2" spans="1:23" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="V2" s="33">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="V2" s="30">
         <f>V3</f>
         <v>1</v>
       </c>
-      <c r="W2" s="33">
+      <c r="W2" s="30">
         <f>-V3</f>
         <v>-1</v>
       </c>
@@ -3394,26 +3394,26 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="32" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="26" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="33">
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="30">
         <f>SUM(M5:M18)</f>
         <v>1</v>
       </c>
-      <c r="W3" s="33">
+      <c r="W3" s="30">
         <f>-V3</f>
         <v>-1</v>
       </c>
@@ -3429,14 +3429,14 @@
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="G4" s="22"/>
+      <c r="I4" s="22"/>
       <c r="M4" s="10" t="s">
         <v>51</v>
       </c>
@@ -4780,7 +4780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -4808,57 +4808,57 @@
       <c r="A1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="30"/>
+      <c r="Y1" s="42"/>
     </row>
     <row r="2" spans="1:31" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="X2" s="33">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="X2" s="30">
         <f>X3</f>
         <v>-1</v>
       </c>
-      <c r="Y2" s="33">
+      <c r="Y2" s="30">
         <f>Y3</f>
         <v>1</v>
       </c>
-      <c r="Z2" s="33">
+      <c r="Z2" s="30">
         <f>X2</f>
         <v>-1</v>
       </c>
-      <c r="AA2" s="31">
+      <c r="AA2" s="28">
         <f>Y2</f>
         <v>1</v>
       </c>
-      <c r="AB2" s="38">
-        <f t="shared" ref="AB2:AB3" si="0">X2</f>
+      <c r="AB2" s="35">
+        <f t="shared" ref="AB2" si="0">X2</f>
         <v>-1</v>
       </c>
-      <c r="AC2" s="39">
+      <c r="AC2" s="36">
         <f>X2</f>
         <v>-1</v>
       </c>
-      <c r="AD2" s="38">
+      <c r="AD2" s="35">
         <f>Y2</f>
         <v>1</v>
       </c>
-      <c r="AE2" s="39">
+      <c r="AE2" s="36">
         <f>Y2</f>
         <v>1</v>
       </c>
@@ -4870,52 +4870,52 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="32" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="26" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="32">
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="29">
         <f>SUM(M5:M18)</f>
         <v>-1</v>
       </c>
-      <c r="Y3" s="33">
+      <c r="Y3" s="30">
         <f>-X3</f>
         <v>1</v>
       </c>
-      <c r="Z3" s="32">
+      <c r="Z3" s="29">
         <f>X3</f>
         <v>-1</v>
       </c>
-      <c r="AA3" s="31">
+      <c r="AA3" s="28">
         <f>Y3</f>
         <v>1</v>
       </c>
-      <c r="AB3" s="40">
+      <c r="AB3" s="37">
         <f>X3</f>
         <v>-1</v>
       </c>
-      <c r="AC3" s="41">
+      <c r="AC3" s="38">
         <f>X3</f>
         <v>-1</v>
       </c>
-      <c r="AD3" s="40">
+      <c r="AD3" s="37">
         <f>Y3</f>
         <v>1</v>
       </c>
-      <c r="AE3" s="41">
+      <c r="AE3" s="38">
         <f>Y3</f>
         <v>1</v>
       </c>
@@ -4931,14 +4931,14 @@
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="G4" s="22"/>
+      <c r="I4" s="22"/>
       <c r="M4" s="10" t="s">
         <v>51</v>
       </c>
@@ -4954,22 +4954,22 @@
       <c r="Q4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="36" t="s">
+      <c r="S4" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="T4" s="36" t="s">
+      <c r="T4" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="37" t="s">
+      <c r="U4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="V4" s="37" t="s">
+      <c r="V4" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="37" t="s">
+      <c r="W4" s="34" t="s">
         <v>64</v>
       </c>
       <c r="X4" s="10" t="s">
@@ -5080,19 +5080,19 @@
         <f>Y5-SUM(Y6:Y9)</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="42">
+      <c r="AB5" s="39">
         <f>X5-B5</f>
         <v>5</v>
       </c>
-      <c r="AC5" s="42">
+      <c r="AC5" s="39">
         <f>C5-X5</f>
         <v>40</v>
       </c>
-      <c r="AD5" s="42">
+      <c r="AD5" s="39">
         <f>Y5-B5</f>
         <v>5</v>
       </c>
-      <c r="AE5" s="42">
+      <c r="AE5" s="39">
         <f>C5-Y5</f>
         <v>40</v>
       </c>
@@ -5144,19 +5144,19 @@
         <f>D6-W6</f>
         <v>1.666666666666667</v>
       </c>
-      <c r="AB6" s="42">
+      <c r="AB6" s="39">
         <f t="shared" ref="AB6:AB20" si="2">X6-B6</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="AC6" s="42">
+      <c r="AC6" s="39">
         <f t="shared" ref="AC6:AC20" si="3">C6-X6</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AD6" s="42">
+      <c r="AD6" s="39">
         <f t="shared" ref="AD6:AD20" si="4">Y6-B6</f>
         <v>1.666666666666667</v>
       </c>
-      <c r="AE6" s="42">
+      <c r="AE6" s="39">
         <f t="shared" ref="AE6:AE20" si="5">C6-Y6</f>
         <v>8.3333333333333321</v>
       </c>
@@ -5204,19 +5204,19 @@
         <f t="shared" ref="Y7:Y20" si="11">D7-W7</f>
         <v>6</v>
       </c>
-      <c r="AB7" s="42">
+      <c r="AB7" s="39">
         <f t="shared" si="2"/>
         <v>0.66666666666666607</v>
       </c>
-      <c r="AC7" s="42">
+      <c r="AC7" s="39">
         <f t="shared" si="3"/>
         <v>9.3333333333333339</v>
       </c>
-      <c r="AD7" s="42">
+      <c r="AD7" s="39">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AE7" s="42">
+      <c r="AE7" s="39">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
@@ -5264,19 +5264,19 @@
         <f t="shared" si="11"/>
         <v>10.666666666666666</v>
       </c>
-      <c r="AB8" s="42">
+      <c r="AB8" s="39">
         <f t="shared" si="2"/>
         <v>-0.66666666666666607</v>
       </c>
-      <c r="AC8" s="42">
+      <c r="AC8" s="39">
         <f t="shared" si="3"/>
         <v>10.666666666666666</v>
       </c>
-      <c r="AD8" s="42">
+      <c r="AD8" s="39">
         <f t="shared" si="4"/>
         <v>0.66666666666666607</v>
       </c>
-      <c r="AE8" s="42">
+      <c r="AE8" s="39">
         <f t="shared" si="5"/>
         <v>9.3333333333333339</v>
       </c>
@@ -5324,19 +5324,19 @@
         <f t="shared" si="11"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="AB9" s="42">
+      <c r="AB9" s="39">
         <f t="shared" si="2"/>
         <v>1.6666666666666679</v>
       </c>
-      <c r="AC9" s="42">
+      <c r="AC9" s="39">
         <f t="shared" si="3"/>
         <v>13.333333333333332</v>
       </c>
-      <c r="AD9" s="42">
+      <c r="AD9" s="39">
         <f t="shared" si="4"/>
         <v>1.6666666666666679</v>
       </c>
-      <c r="AE9" s="42">
+      <c r="AE9" s="39">
         <f t="shared" si="5"/>
         <v>13.333333333333332</v>
       </c>
@@ -5419,19 +5419,19 @@
         <f>Y10-SUM(Y11:Y13)</f>
         <v>0</v>
       </c>
-      <c r="AB10" s="42">
+      <c r="AB10" s="39">
         <f t="shared" si="2"/>
         <v>26.666666666666664</v>
       </c>
-      <c r="AC10" s="42">
+      <c r="AC10" s="39">
         <f t="shared" si="3"/>
         <v>0.3333333333333357</v>
       </c>
-      <c r="AD10" s="42">
+      <c r="AD10" s="39">
         <f t="shared" si="4"/>
         <v>20.804597701149426</v>
       </c>
-      <c r="AE10" s="42">
+      <c r="AE10" s="39">
         <f t="shared" si="5"/>
         <v>6.1954022988505741</v>
       </c>
@@ -5483,19 +5483,19 @@
         <f t="shared" si="11"/>
         <v>6.4597701149425291</v>
       </c>
-      <c r="AB11" s="42">
+      <c r="AB11" s="39">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AC11" s="42">
+      <c r="AC11" s="39">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="AD11" s="42">
+      <c r="AD11" s="39">
         <f t="shared" si="4"/>
         <v>6.4597701149425291</v>
       </c>
-      <c r="AE11" s="42">
+      <c r="AE11" s="39">
         <f t="shared" si="5"/>
         <v>3.5402298850574709</v>
       </c>
@@ -5543,19 +5543,19 @@
         <f t="shared" si="11"/>
         <v>24.114942528735632</v>
       </c>
-      <c r="AB12" s="42">
+      <c r="AB12" s="39">
         <f t="shared" si="2"/>
         <v>18.666666666666664</v>
       </c>
-      <c r="AC12" s="42">
+      <c r="AC12" s="39">
         <f t="shared" si="3"/>
         <v>-3.6666666666666643</v>
       </c>
-      <c r="AD12" s="42">
+      <c r="AD12" s="39">
         <f t="shared" si="4"/>
         <v>14.114942528735632</v>
       </c>
-      <c r="AE12" s="42">
+      <c r="AE12" s="39">
         <f t="shared" si="5"/>
         <v>0.88505747126436773</v>
       </c>
@@ -5603,19 +5603,19 @@
         <f t="shared" si="11"/>
         <v>5.2298850574712645</v>
       </c>
-      <c r="AB13" s="42">
+      <c r="AB13" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC13" s="42">
+      <c r="AC13" s="39">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="AD13" s="42">
+      <c r="AD13" s="39">
         <f t="shared" si="4"/>
         <v>0.22988505747126453</v>
       </c>
-      <c r="AE13" s="42">
+      <c r="AE13" s="39">
         <f t="shared" si="5"/>
         <v>1.7701149425287355</v>
       </c>
@@ -5698,19 +5698,19 @@
         <f>Y14-SUM(Y15:Y17)</f>
         <v>0</v>
       </c>
-      <c r="AB14" s="42">
+      <c r="AB14" s="39">
         <f t="shared" si="2"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC14" s="42">
+      <c r="AC14" s="39">
         <f t="shared" si="3"/>
         <v>38.333333333333336</v>
       </c>
-      <c r="AD14" s="42">
+      <c r="AD14" s="39">
         <f t="shared" si="4"/>
         <v>9.5977011494252871</v>
       </c>
-      <c r="AE14" s="42">
+      <c r="AE14" s="39">
         <f t="shared" si="5"/>
         <v>35.402298850574709</v>
       </c>
@@ -5762,19 +5762,19 @@
         <f t="shared" si="11"/>
         <v>8.1839080459770113</v>
       </c>
-      <c r="AB15" s="42">
+      <c r="AB15" s="39">
         <f t="shared" si="2"/>
         <v>1.333333333333333</v>
       </c>
-      <c r="AC15" s="42">
+      <c r="AC15" s="39">
         <f t="shared" si="3"/>
         <v>18.666666666666668</v>
       </c>
-      <c r="AD15" s="42">
+      <c r="AD15" s="39">
         <f t="shared" si="4"/>
         <v>3.1839080459770113</v>
       </c>
-      <c r="AE15" s="42">
+      <c r="AE15" s="39">
         <f t="shared" si="5"/>
         <v>16.816091954022987</v>
       </c>
@@ -5822,19 +5822,19 @@
         <f t="shared" si="11"/>
         <v>1.7241379310344827</v>
       </c>
-      <c r="AB16" s="42">
+      <c r="AB16" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC16" s="42">
+      <c r="AC16" s="39">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="AD16" s="42">
+      <c r="AD16" s="39">
         <f t="shared" si="4"/>
         <v>1.7241379310344827</v>
       </c>
-      <c r="AE16" s="42">
+      <c r="AE16" s="39">
         <f t="shared" si="5"/>
         <v>13.275862068965518</v>
       </c>
@@ -5882,19 +5882,19 @@
         <f t="shared" si="11"/>
         <v>4.6896551724137936</v>
       </c>
-      <c r="AB17" s="42">
+      <c r="AB17" s="39">
         <f t="shared" si="2"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="AC17" s="42">
+      <c r="AC17" s="39">
         <f t="shared" si="3"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="AD17" s="42">
+      <c r="AD17" s="39">
         <f t="shared" si="4"/>
         <v>4.6896551724137936</v>
       </c>
-      <c r="AE17" s="42">
+      <c r="AE17" s="39">
         <f t="shared" si="5"/>
         <v>5.3103448275862064</v>
       </c>
@@ -5977,19 +5977,19 @@
         <f>Y18-SUM(Y19:Y20)</f>
         <v>0</v>
       </c>
-      <c r="AB18" s="42">
+      <c r="AB18" s="39">
         <f t="shared" si="2"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC18" s="42">
+      <c r="AC18" s="39">
         <f t="shared" si="3"/>
         <v>38.333333333333336</v>
       </c>
-      <c r="AD18" s="42">
+      <c r="AD18" s="39">
         <f t="shared" si="4"/>
         <v>9.5977011494252871</v>
       </c>
-      <c r="AE18" s="42">
+      <c r="AE18" s="39">
         <f t="shared" si="5"/>
         <v>35.402298850574709</v>
       </c>
@@ -6041,19 +6041,19 @@
         <f t="shared" si="11"/>
         <v>7.8735632183908049</v>
       </c>
-      <c r="AB19" s="42">
+      <c r="AB19" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC19" s="42">
+      <c r="AC19" s="39">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="AD19" s="42">
+      <c r="AD19" s="39">
         <f t="shared" si="4"/>
         <v>2.8735632183908049</v>
       </c>
-      <c r="AE19" s="42">
+      <c r="AE19" s="39">
         <f t="shared" si="5"/>
         <v>22.126436781609193</v>
       </c>
@@ -6101,19 +6101,19 @@
         <f t="shared" si="11"/>
         <v>6.7241379310344822</v>
       </c>
-      <c r="AB20" s="42">
+      <c r="AB20" s="39">
         <f t="shared" si="2"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="AC20" s="42">
+      <c r="AC20" s="39">
         <f t="shared" si="3"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="AD20" s="42">
+      <c r="AD20" s="39">
         <f t="shared" si="4"/>
         <v>6.7241379310344822</v>
       </c>
-      <c r="AE20" s="42">
+      <c r="AE20" s="39">
         <f t="shared" si="5"/>
         <v>13.275862068965518</v>
       </c>

</xml_diff>

<commit_message>
intermediary preparation for charts
</commit_message>
<xml_diff>
--- a/Algorithm to control changes in weight.xlsx
+++ b/Algorithm to control changes in weight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="15" r:id="rId1"/>
@@ -2647,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="X7" sqref="X7"/>

</xml_diff>